<commit_message>
Export model responses for checking, and filter eval results by valid questions only (from excel sheets)
</commit_message>
<xml_diff>
--- a/data/annotation/product_cq.xlsx
+++ b/data/annotation/product_cq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuchaoqun/Documents/Projects/RAG_MM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiayewken/Downloads/Projects/Work/MultimodalFinance/data/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857D9EBE-8DB1-8140-AFD6-B39CFC18EB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEF2CDB-B224-274A-BF94-A1C471B9FFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="728">
   <si>
     <t>data_file</t>
   </si>
@@ -2264,6 +2261,9 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>valid</t>
   </si>
 </sst>
 </file>
@@ -2348,9 +2348,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2361,6 +2358,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2663,12 +2663,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L355"/>
+  <dimension ref="A1:M355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I265" sqref="I265"/>
+      <selection pane="bottomLeft" activeCell="O292" sqref="O292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2677,15 +2677,15 @@
     <col min="2" max="2" width="18.1640625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="112.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="112.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" customWidth="1"/>
     <col min="10" max="10" width="21.33203125" customWidth="1"/>
     <col min="11" max="11" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2701,10 +2701,10 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>718</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -2719,11 +2719,14 @@
       <c r="K1" s="2" t="s">
         <v>723</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="20" x14ac:dyDescent="0.25">
+      <c r="M1" s="7" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2739,11 +2742,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2759,11 +2762,11 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2779,11 +2782,11 @@
       <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2799,11 +2802,11 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2819,11 +2822,11 @@
       <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2839,11 +2842,11 @@
       <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2859,11 +2862,11 @@
       <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2879,11 +2882,11 @@
       <c r="E9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2899,11 +2902,11 @@
       <c r="E10" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2919,11 +2922,11 @@
       <c r="E11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="80" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2939,11 +2942,11 @@
       <c r="E12" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -2959,11 +2962,11 @@
       <c r="E13" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2979,11 +2982,11 @@
       <c r="E14" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2999,11 +3002,11 @@
       <c r="E15" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -3019,7 +3022,7 @@
       <c r="E16" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3039,7 +3042,7 @@
       <c r="E17" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3059,7 +3062,7 @@
       <c r="E18" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3079,7 +3082,7 @@
       <c r="E19" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3099,7 +3102,7 @@
       <c r="E20" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3119,7 +3122,7 @@
       <c r="E21" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3139,7 +3142,7 @@
       <c r="E22" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3159,7 +3162,7 @@
       <c r="E23" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3179,7 +3182,7 @@
       <c r="E24" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3199,7 +3202,7 @@
       <c r="E25" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3219,7 +3222,7 @@
       <c r="E26" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3239,7 +3242,7 @@
       <c r="E27" t="s">
         <v>60</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="4" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3259,7 +3262,7 @@
       <c r="E28" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3279,7 +3282,7 @@
       <c r="E29" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3299,7 +3302,7 @@
       <c r="E30" t="s">
         <v>66</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3319,7 +3322,7 @@
       <c r="E31" t="s">
         <v>68</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3339,7 +3342,7 @@
       <c r="E32" t="s">
         <v>70</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3359,7 +3362,7 @@
       <c r="E33" t="s">
         <v>72</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="4" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3379,7 +3382,7 @@
       <c r="E34" t="s">
         <v>74</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="4" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3399,7 +3402,7 @@
       <c r="E35" t="s">
         <v>76</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3419,7 +3422,7 @@
       <c r="E36" t="s">
         <v>78</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="4" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3439,7 +3442,7 @@
       <c r="E37" t="s">
         <v>80</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="4" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3459,7 +3462,7 @@
       <c r="E38" t="s">
         <v>82</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="4" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3479,7 +3482,7 @@
       <c r="E39" t="s">
         <v>84</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="4" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3499,7 +3502,7 @@
       <c r="E40" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F40" s="4" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3519,7 +3522,7 @@
       <c r="E41" t="s">
         <v>88</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="4" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3539,7 +3542,7 @@
       <c r="E42" t="s">
         <v>90</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3559,7 +3562,7 @@
       <c r="E43" t="s">
         <v>92</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3579,7 +3582,7 @@
       <c r="E44" t="s">
         <v>94</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F44" s="4" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3599,7 +3602,7 @@
       <c r="E45" t="s">
         <v>96</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="F45" s="4" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3619,7 +3622,7 @@
       <c r="E46" t="s">
         <v>98</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="4" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3639,7 +3642,7 @@
       <c r="E47" t="s">
         <v>100</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3659,7 +3662,7 @@
       <c r="E48" t="s">
         <v>102</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3679,7 +3682,7 @@
       <c r="E49" t="s">
         <v>104</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="4" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3699,7 +3702,7 @@
       <c r="E50" t="s">
         <v>106</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F50" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3719,7 +3722,7 @@
       <c r="E51" t="s">
         <v>108</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F51" s="4" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3739,7 +3742,7 @@
       <c r="E52" t="s">
         <v>110</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F52" s="4" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3759,7 +3762,7 @@
       <c r="E53" t="s">
         <v>112</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="F53" s="4" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3779,7 +3782,7 @@
       <c r="E54" t="s">
         <v>114</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="4" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3799,7 +3802,7 @@
       <c r="E55" t="s">
         <v>116</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="F55" s="4" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3819,7 +3822,7 @@
       <c r="E56" t="s">
         <v>118</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="4" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3839,7 +3842,7 @@
       <c r="E57" t="s">
         <v>120</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F57" s="4" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3859,7 +3862,7 @@
       <c r="E58" t="s">
         <v>122</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="4" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3879,7 +3882,7 @@
       <c r="E59" t="s">
         <v>124</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F59" s="4" t="s">
         <v>125</v>
       </c>
     </row>
@@ -3899,7 +3902,7 @@
       <c r="E60" t="s">
         <v>126</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" s="4" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3919,7 +3922,7 @@
       <c r="E61" t="s">
         <v>128</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="4" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3939,7 +3942,7 @@
       <c r="E62" t="s">
         <v>130</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="4" t="s">
         <v>131</v>
       </c>
     </row>
@@ -3959,7 +3962,7 @@
       <c r="E63" t="s">
         <v>132</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="4" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3979,7 +3982,7 @@
       <c r="E64" t="s">
         <v>134</v>
       </c>
-      <c r="F64" s="5" t="s">
+      <c r="F64" s="4" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3999,7 +4002,7 @@
       <c r="E65" t="s">
         <v>136</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="F65" s="4" t="s">
         <v>137</v>
       </c>
     </row>
@@ -4019,7 +4022,7 @@
       <c r="E66" t="s">
         <v>138</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="4" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4039,7 +4042,7 @@
       <c r="E67" t="s">
         <v>140</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F67" s="4" t="s">
         <v>141</v>
       </c>
     </row>
@@ -4059,7 +4062,7 @@
       <c r="E68" t="s">
         <v>142</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="4" t="s">
         <v>143</v>
       </c>
     </row>
@@ -4079,7 +4082,7 @@
       <c r="E69" t="s">
         <v>144</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="F69" s="4" t="s">
         <v>145</v>
       </c>
     </row>
@@ -4099,7 +4102,7 @@
       <c r="E70" t="s">
         <v>146</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="F70" s="4" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4119,7 +4122,7 @@
       <c r="E71" t="s">
         <v>148</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F71" s="4" t="s">
         <v>149</v>
       </c>
     </row>
@@ -4139,7 +4142,7 @@
       <c r="E72" t="s">
         <v>150</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F72" s="4" t="s">
         <v>151</v>
       </c>
     </row>
@@ -4159,7 +4162,7 @@
       <c r="E73" t="s">
         <v>152</v>
       </c>
-      <c r="F73" s="5" t="s">
+      <c r="F73" s="4" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4179,7 +4182,7 @@
       <c r="E74" t="s">
         <v>154</v>
       </c>
-      <c r="F74" s="5" t="s">
+      <c r="F74" s="4" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4199,7 +4202,7 @@
       <c r="E75" t="s">
         <v>156</v>
       </c>
-      <c r="F75" s="5" t="s">
+      <c r="F75" s="4" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4219,7 +4222,7 @@
       <c r="E76" t="s">
         <v>158</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F76" s="4" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4239,7 +4242,7 @@
       <c r="E77" t="s">
         <v>160</v>
       </c>
-      <c r="F77" s="5" t="s">
+      <c r="F77" s="4" t="s">
         <v>161</v>
       </c>
     </row>
@@ -4259,7 +4262,7 @@
       <c r="E78" t="s">
         <v>162</v>
       </c>
-      <c r="F78" s="5" t="s">
+      <c r="F78" s="4" t="s">
         <v>163</v>
       </c>
     </row>
@@ -4279,7 +4282,7 @@
       <c r="E79" t="s">
         <v>164</v>
       </c>
-      <c r="F79" s="5" t="s">
+      <c r="F79" s="4" t="s">
         <v>165</v>
       </c>
     </row>
@@ -4299,7 +4302,7 @@
       <c r="E80" t="s">
         <v>166</v>
       </c>
-      <c r="F80" s="5" t="s">
+      <c r="F80" s="4" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4319,7 +4322,7 @@
       <c r="E81" t="s">
         <v>168</v>
       </c>
-      <c r="F81" s="5" t="s">
+      <c r="F81" s="4" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4339,7 +4342,7 @@
       <c r="E82" t="s">
         <v>170</v>
       </c>
-      <c r="F82" s="5" t="s">
+      <c r="F82" s="4" t="s">
         <v>171</v>
       </c>
     </row>
@@ -4359,7 +4362,7 @@
       <c r="E83" t="s">
         <v>172</v>
       </c>
-      <c r="F83" s="5" t="s">
+      <c r="F83" s="4" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4379,7 +4382,7 @@
       <c r="E84" t="s">
         <v>174</v>
       </c>
-      <c r="F84" s="5" t="s">
+      <c r="F84" s="4" t="s">
         <v>175</v>
       </c>
     </row>
@@ -4399,7 +4402,7 @@
       <c r="E85" t="s">
         <v>176</v>
       </c>
-      <c r="F85" s="5" t="s">
+      <c r="F85" s="4" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4419,7 +4422,7 @@
       <c r="E86" t="s">
         <v>178</v>
       </c>
-      <c r="F86" s="5" t="s">
+      <c r="F86" s="4" t="s">
         <v>179</v>
       </c>
     </row>
@@ -4439,7 +4442,7 @@
       <c r="E87" t="s">
         <v>180</v>
       </c>
-      <c r="F87" s="5" t="s">
+      <c r="F87" s="4" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4459,7 +4462,7 @@
       <c r="E88" t="s">
         <v>182</v>
       </c>
-      <c r="F88" s="5" t="s">
+      <c r="F88" s="4" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4479,7 +4482,7 @@
       <c r="E89" t="s">
         <v>184</v>
       </c>
-      <c r="F89" s="5" t="s">
+      <c r="F89" s="4" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4499,7 +4502,7 @@
       <c r="E90" t="s">
         <v>186</v>
       </c>
-      <c r="F90" s="5" t="s">
+      <c r="F90" s="4" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4519,7 +4522,7 @@
       <c r="E91" t="s">
         <v>188</v>
       </c>
-      <c r="F91" s="5" t="s">
+      <c r="F91" s="4" t="s">
         <v>189</v>
       </c>
     </row>
@@ -4539,7 +4542,7 @@
       <c r="E92" t="s">
         <v>190</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="F92" s="4" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4559,7 +4562,7 @@
       <c r="E93" t="s">
         <v>192</v>
       </c>
-      <c r="F93" s="5" t="s">
+      <c r="F93" s="4" t="s">
         <v>193</v>
       </c>
     </row>
@@ -4579,7 +4582,7 @@
       <c r="E94" t="s">
         <v>194</v>
       </c>
-      <c r="F94" s="5" t="s">
+      <c r="F94" s="4" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4599,7 +4602,7 @@
       <c r="E95" t="s">
         <v>196</v>
       </c>
-      <c r="F95" s="5" t="s">
+      <c r="F95" s="4" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4619,7 +4622,7 @@
       <c r="E96" t="s">
         <v>198</v>
       </c>
-      <c r="F96" s="5" t="s">
+      <c r="F96" s="4" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4639,7 +4642,7 @@
       <c r="E97" t="s">
         <v>200</v>
       </c>
-      <c r="F97" s="5" t="s">
+      <c r="F97" s="4" t="s">
         <v>201</v>
       </c>
     </row>
@@ -4659,7 +4662,7 @@
       <c r="E98" t="s">
         <v>202</v>
       </c>
-      <c r="F98" s="5" t="s">
+      <c r="F98" s="4" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4679,7 +4682,7 @@
       <c r="E99" t="s">
         <v>204</v>
       </c>
-      <c r="F99" s="5" t="s">
+      <c r="F99" s="4" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4699,7 +4702,7 @@
       <c r="E100" t="s">
         <v>206</v>
       </c>
-      <c r="F100" s="5" t="s">
+      <c r="F100" s="4" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4719,7 +4722,7 @@
       <c r="E101" t="s">
         <v>208</v>
       </c>
-      <c r="F101" s="5" t="s">
+      <c r="F101" s="4" t="s">
         <v>209</v>
       </c>
     </row>
@@ -4739,7 +4742,7 @@
       <c r="E102" t="s">
         <v>210</v>
       </c>
-      <c r="F102" s="5" t="s">
+      <c r="F102" s="4" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4759,7 +4762,7 @@
       <c r="E103" t="s">
         <v>212</v>
       </c>
-      <c r="F103" s="5" t="s">
+      <c r="F103" s="4" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4779,7 +4782,7 @@
       <c r="E104" t="s">
         <v>214</v>
       </c>
-      <c r="F104" s="5" t="s">
+      <c r="F104" s="4" t="s">
         <v>215</v>
       </c>
     </row>
@@ -4799,7 +4802,7 @@
       <c r="E105" t="s">
         <v>216</v>
       </c>
-      <c r="F105" s="5" t="s">
+      <c r="F105" s="4" t="s">
         <v>217</v>
       </c>
     </row>
@@ -4819,7 +4822,7 @@
       <c r="E106" t="s">
         <v>218</v>
       </c>
-      <c r="F106" s="5" t="s">
+      <c r="F106" s="4" t="s">
         <v>219</v>
       </c>
     </row>
@@ -4839,7 +4842,7 @@
       <c r="E107" t="s">
         <v>220</v>
       </c>
-      <c r="F107" s="5" t="s">
+      <c r="F107" s="4" t="s">
         <v>221</v>
       </c>
     </row>
@@ -4859,7 +4862,7 @@
       <c r="E108" t="s">
         <v>222</v>
       </c>
-      <c r="F108" s="5" t="s">
+      <c r="F108" s="4" t="s">
         <v>223</v>
       </c>
     </row>
@@ -4879,7 +4882,7 @@
       <c r="E109" t="s">
         <v>224</v>
       </c>
-      <c r="F109" s="5" t="s">
+      <c r="F109" s="4" t="s">
         <v>225</v>
       </c>
     </row>
@@ -4899,7 +4902,7 @@
       <c r="E110" t="s">
         <v>226</v>
       </c>
-      <c r="F110" s="5" t="s">
+      <c r="F110" s="4" t="s">
         <v>227</v>
       </c>
     </row>
@@ -4919,7 +4922,7 @@
       <c r="E111" t="s">
         <v>228</v>
       </c>
-      <c r="F111" s="5" t="s">
+      <c r="F111" s="4" t="s">
         <v>229</v>
       </c>
     </row>
@@ -4939,7 +4942,7 @@
       <c r="E112" t="s">
         <v>230</v>
       </c>
-      <c r="F112" s="5" t="s">
+      <c r="F112" s="4" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4959,7 +4962,7 @@
       <c r="E113" t="s">
         <v>232</v>
       </c>
-      <c r="F113" s="5" t="s">
+      <c r="F113" s="4" t="s">
         <v>233</v>
       </c>
     </row>
@@ -4979,7 +4982,7 @@
       <c r="E114" t="s">
         <v>234</v>
       </c>
-      <c r="F114" s="5" t="s">
+      <c r="F114" s="4" t="s">
         <v>235</v>
       </c>
     </row>
@@ -4999,7 +5002,7 @@
       <c r="E115" t="s">
         <v>236</v>
       </c>
-      <c r="F115" s="5" t="s">
+      <c r="F115" s="4" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5019,7 +5022,7 @@
       <c r="E116" t="s">
         <v>238</v>
       </c>
-      <c r="F116" s="5" t="s">
+      <c r="F116" s="4" t="s">
         <v>239</v>
       </c>
     </row>
@@ -5039,7 +5042,7 @@
       <c r="E117" t="s">
         <v>240</v>
       </c>
-      <c r="F117" s="5" t="s">
+      <c r="F117" s="4" t="s">
         <v>241</v>
       </c>
     </row>
@@ -5059,7 +5062,7 @@
       <c r="E118" t="s">
         <v>242</v>
       </c>
-      <c r="F118" s="5" t="s">
+      <c r="F118" s="4" t="s">
         <v>243</v>
       </c>
     </row>
@@ -5079,7 +5082,7 @@
       <c r="E119" t="s">
         <v>244</v>
       </c>
-      <c r="F119" s="5" t="s">
+      <c r="F119" s="4" t="s">
         <v>245</v>
       </c>
     </row>
@@ -5099,7 +5102,7 @@
       <c r="E120" t="s">
         <v>246</v>
       </c>
-      <c r="F120" s="5" t="s">
+      <c r="F120" s="4" t="s">
         <v>247</v>
       </c>
     </row>
@@ -5119,7 +5122,7 @@
       <c r="E121" t="s">
         <v>248</v>
       </c>
-      <c r="F121" s="5" t="s">
+      <c r="F121" s="4" t="s">
         <v>249</v>
       </c>
     </row>
@@ -5139,7 +5142,7 @@
       <c r="E122" t="s">
         <v>250</v>
       </c>
-      <c r="F122" s="5" t="s">
+      <c r="F122" s="4" t="s">
         <v>251</v>
       </c>
     </row>
@@ -5159,7 +5162,7 @@
       <c r="E123" t="s">
         <v>252</v>
       </c>
-      <c r="F123" s="5" t="s">
+      <c r="F123" s="4" t="s">
         <v>253</v>
       </c>
     </row>
@@ -5179,7 +5182,7 @@
       <c r="E124" t="s">
         <v>254</v>
       </c>
-      <c r="F124" s="5" t="s">
+      <c r="F124" s="4" t="s">
         <v>255</v>
       </c>
     </row>
@@ -5199,7 +5202,7 @@
       <c r="E125" t="s">
         <v>256</v>
       </c>
-      <c r="F125" s="5" t="s">
+      <c r="F125" s="4" t="s">
         <v>257</v>
       </c>
     </row>
@@ -5219,7 +5222,7 @@
       <c r="E126" t="s">
         <v>258</v>
       </c>
-      <c r="F126" s="5" t="s">
+      <c r="F126" s="4" t="s">
         <v>259</v>
       </c>
     </row>
@@ -5239,7 +5242,7 @@
       <c r="E127" t="s">
         <v>260</v>
       </c>
-      <c r="F127" s="5" t="s">
+      <c r="F127" s="4" t="s">
         <v>261</v>
       </c>
     </row>
@@ -5259,7 +5262,7 @@
       <c r="E128" t="s">
         <v>262</v>
       </c>
-      <c r="F128" s="5" t="s">
+      <c r="F128" s="4" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5279,7 +5282,7 @@
       <c r="E129" t="s">
         <v>264</v>
       </c>
-      <c r="F129" s="5" t="s">
+      <c r="F129" s="4" t="s">
         <v>265</v>
       </c>
     </row>
@@ -5299,7 +5302,7 @@
       <c r="E130" t="s">
         <v>266</v>
       </c>
-      <c r="F130" s="5" t="s">
+      <c r="F130" s="4" t="s">
         <v>267</v>
       </c>
     </row>
@@ -5319,7 +5322,7 @@
       <c r="E131" t="s">
         <v>268</v>
       </c>
-      <c r="F131" s="5" t="s">
+      <c r="F131" s="4" t="s">
         <v>269</v>
       </c>
     </row>
@@ -5339,7 +5342,7 @@
       <c r="E132" t="s">
         <v>270</v>
       </c>
-      <c r="F132" s="5" t="s">
+      <c r="F132" s="4" t="s">
         <v>271</v>
       </c>
     </row>
@@ -5359,7 +5362,7 @@
       <c r="E133" t="s">
         <v>272</v>
       </c>
-      <c r="F133" s="5" t="s">
+      <c r="F133" s="4" t="s">
         <v>273</v>
       </c>
     </row>
@@ -5379,7 +5382,7 @@
       <c r="E134" t="s">
         <v>274</v>
       </c>
-      <c r="F134" s="5" t="s">
+      <c r="F134" s="4" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5399,7 +5402,7 @@
       <c r="E135" t="s">
         <v>276</v>
       </c>
-      <c r="F135" s="5" t="s">
+      <c r="F135" s="4" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5419,7 +5422,7 @@
       <c r="E136" t="s">
         <v>278</v>
       </c>
-      <c r="F136" s="5" t="s">
+      <c r="F136" s="4" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5439,7 +5442,7 @@
       <c r="E137" t="s">
         <v>280</v>
       </c>
-      <c r="F137" s="5" t="s">
+      <c r="F137" s="4" t="s">
         <v>281</v>
       </c>
     </row>
@@ -5459,7 +5462,7 @@
       <c r="E138" t="s">
         <v>282</v>
       </c>
-      <c r="F138" s="5" t="s">
+      <c r="F138" s="4" t="s">
         <v>283</v>
       </c>
     </row>
@@ -5479,7 +5482,7 @@
       <c r="E139" t="s">
         <v>284</v>
       </c>
-      <c r="F139" s="5" t="s">
+      <c r="F139" s="4" t="s">
         <v>285</v>
       </c>
     </row>
@@ -5499,7 +5502,7 @@
       <c r="E140" t="s">
         <v>286</v>
       </c>
-      <c r="F140" s="5" t="s">
+      <c r="F140" s="4" t="s">
         <v>287</v>
       </c>
     </row>
@@ -5519,7 +5522,7 @@
       <c r="E141" t="s">
         <v>288</v>
       </c>
-      <c r="F141" s="5" t="s">
+      <c r="F141" s="4" t="s">
         <v>289</v>
       </c>
     </row>
@@ -5539,7 +5542,7 @@
       <c r="E142" t="s">
         <v>290</v>
       </c>
-      <c r="F142" s="5" t="s">
+      <c r="F142" s="4" t="s">
         <v>291</v>
       </c>
     </row>
@@ -5559,7 +5562,7 @@
       <c r="E143" t="s">
         <v>292</v>
       </c>
-      <c r="F143" s="5" t="s">
+      <c r="F143" s="4" t="s">
         <v>293</v>
       </c>
     </row>
@@ -5579,7 +5582,7 @@
       <c r="E144" t="s">
         <v>294</v>
       </c>
-      <c r="F144" s="5" t="s">
+      <c r="F144" s="4" t="s">
         <v>295</v>
       </c>
     </row>
@@ -5599,7 +5602,7 @@
       <c r="E145" t="s">
         <v>296</v>
       </c>
-      <c r="F145" s="5" t="s">
+      <c r="F145" s="4" t="s">
         <v>297</v>
       </c>
     </row>
@@ -5619,7 +5622,7 @@
       <c r="E146" t="s">
         <v>298</v>
       </c>
-      <c r="F146" s="5" t="s">
+      <c r="F146" s="4" t="s">
         <v>299</v>
       </c>
     </row>
@@ -5639,7 +5642,7 @@
       <c r="E147" t="s">
         <v>300</v>
       </c>
-      <c r="F147" s="5" t="s">
+      <c r="F147" s="4" t="s">
         <v>301</v>
       </c>
     </row>
@@ -5659,7 +5662,7 @@
       <c r="E148" t="s">
         <v>302</v>
       </c>
-      <c r="F148" s="5" t="s">
+      <c r="F148" s="4" t="s">
         <v>303</v>
       </c>
     </row>
@@ -5679,7 +5682,7 @@
       <c r="E149" t="s">
         <v>304</v>
       </c>
-      <c r="F149" s="5" t="s">
+      <c r="F149" s="4" t="s">
         <v>305</v>
       </c>
     </row>
@@ -5699,7 +5702,7 @@
       <c r="E150" t="s">
         <v>306</v>
       </c>
-      <c r="F150" s="5" t="s">
+      <c r="F150" s="4" t="s">
         <v>307</v>
       </c>
     </row>
@@ -5719,7 +5722,7 @@
       <c r="E151" t="s">
         <v>308</v>
       </c>
-      <c r="F151" s="5" t="s">
+      <c r="F151" s="4" t="s">
         <v>309</v>
       </c>
     </row>
@@ -5739,7 +5742,7 @@
       <c r="E152" t="s">
         <v>310</v>
       </c>
-      <c r="F152" s="5" t="s">
+      <c r="F152" s="4" t="s">
         <v>311</v>
       </c>
     </row>
@@ -5759,7 +5762,7 @@
       <c r="E153" t="s">
         <v>312</v>
       </c>
-      <c r="F153" s="5" t="s">
+      <c r="F153" s="4" t="s">
         <v>313</v>
       </c>
     </row>
@@ -5779,7 +5782,7 @@
       <c r="E154" t="s">
         <v>314</v>
       </c>
-      <c r="F154" s="5" t="s">
+      <c r="F154" s="4" t="s">
         <v>315</v>
       </c>
     </row>
@@ -5799,7 +5802,7 @@
       <c r="E155" t="s">
         <v>316</v>
       </c>
-      <c r="F155" s="5" t="s">
+      <c r="F155" s="4" t="s">
         <v>317</v>
       </c>
     </row>
@@ -5819,7 +5822,7 @@
       <c r="E156" t="s">
         <v>318</v>
       </c>
-      <c r="F156" s="5" t="s">
+      <c r="F156" s="4" t="s">
         <v>319</v>
       </c>
     </row>
@@ -5839,7 +5842,7 @@
       <c r="E157" t="s">
         <v>320</v>
       </c>
-      <c r="F157" s="5" t="s">
+      <c r="F157" s="4" t="s">
         <v>321</v>
       </c>
     </row>
@@ -5859,7 +5862,7 @@
       <c r="E158" t="s">
         <v>322</v>
       </c>
-      <c r="F158" s="5" t="s">
+      <c r="F158" s="4" t="s">
         <v>323</v>
       </c>
     </row>
@@ -5879,7 +5882,7 @@
       <c r="E159" t="s">
         <v>324</v>
       </c>
-      <c r="F159" s="5" t="s">
+      <c r="F159" s="4" t="s">
         <v>325</v>
       </c>
     </row>
@@ -5899,7 +5902,7 @@
       <c r="E160" t="s">
         <v>326</v>
       </c>
-      <c r="F160" s="5" t="s">
+      <c r="F160" s="4" t="s">
         <v>327</v>
       </c>
     </row>
@@ -5919,7 +5922,7 @@
       <c r="E161" t="s">
         <v>328</v>
       </c>
-      <c r="F161" s="5" t="s">
+      <c r="F161" s="4" t="s">
         <v>329</v>
       </c>
     </row>
@@ -5939,7 +5942,7 @@
       <c r="E162" t="s">
         <v>330</v>
       </c>
-      <c r="F162" s="5" t="s">
+      <c r="F162" s="4" t="s">
         <v>331</v>
       </c>
     </row>
@@ -5959,7 +5962,7 @@
       <c r="E163" t="s">
         <v>332</v>
       </c>
-      <c r="F163" s="5" t="s">
+      <c r="F163" s="4" t="s">
         <v>333</v>
       </c>
     </row>
@@ -5979,7 +5982,7 @@
       <c r="E164" t="s">
         <v>334</v>
       </c>
-      <c r="F164" s="5" t="s">
+      <c r="F164" s="4" t="s">
         <v>335</v>
       </c>
     </row>
@@ -5999,7 +6002,7 @@
       <c r="E165" t="s">
         <v>336</v>
       </c>
-      <c r="F165" s="5" t="s">
+      <c r="F165" s="4" t="s">
         <v>337</v>
       </c>
     </row>
@@ -6019,7 +6022,7 @@
       <c r="E166" t="s">
         <v>338</v>
       </c>
-      <c r="F166" s="5" t="s">
+      <c r="F166" s="4" t="s">
         <v>339</v>
       </c>
     </row>
@@ -6039,7 +6042,7 @@
       <c r="E167" t="s">
         <v>340</v>
       </c>
-      <c r="F167" s="5" t="s">
+      <c r="F167" s="4" t="s">
         <v>341</v>
       </c>
     </row>
@@ -6059,7 +6062,7 @@
       <c r="E168" t="s">
         <v>342</v>
       </c>
-      <c r="F168" s="5" t="s">
+      <c r="F168" s="4" t="s">
         <v>343</v>
       </c>
     </row>
@@ -6079,7 +6082,7 @@
       <c r="E169" t="s">
         <v>344</v>
       </c>
-      <c r="F169" s="5" t="s">
+      <c r="F169" s="4" t="s">
         <v>345</v>
       </c>
     </row>
@@ -6099,7 +6102,7 @@
       <c r="E170" t="s">
         <v>346</v>
       </c>
-      <c r="F170" s="5" t="s">
+      <c r="F170" s="4" t="s">
         <v>347</v>
       </c>
     </row>
@@ -6119,7 +6122,7 @@
       <c r="E171" t="s">
         <v>348</v>
       </c>
-      <c r="F171" s="5" t="s">
+      <c r="F171" s="4" t="s">
         <v>349</v>
       </c>
     </row>
@@ -6139,7 +6142,7 @@
       <c r="E172" t="s">
         <v>350</v>
       </c>
-      <c r="F172" s="5" t="s">
+      <c r="F172" s="4" t="s">
         <v>351</v>
       </c>
     </row>
@@ -6159,7 +6162,7 @@
       <c r="E173" t="s">
         <v>352</v>
       </c>
-      <c r="F173" s="5" t="s">
+      <c r="F173" s="4" t="s">
         <v>353</v>
       </c>
     </row>
@@ -6179,7 +6182,7 @@
       <c r="E174" t="s">
         <v>354</v>
       </c>
-      <c r="F174" s="5" t="s">
+      <c r="F174" s="4" t="s">
         <v>355</v>
       </c>
     </row>
@@ -6199,7 +6202,7 @@
       <c r="E175" t="s">
         <v>356</v>
       </c>
-      <c r="F175" s="5" t="s">
+      <c r="F175" s="4" t="s">
         <v>357</v>
       </c>
     </row>
@@ -6219,7 +6222,7 @@
       <c r="E176" t="s">
         <v>358</v>
       </c>
-      <c r="F176" s="5" t="s">
+      <c r="F176" s="4" t="s">
         <v>359</v>
       </c>
     </row>
@@ -6239,7 +6242,7 @@
       <c r="E177" t="s">
         <v>360</v>
       </c>
-      <c r="F177" s="5" t="s">
+      <c r="F177" s="4" t="s">
         <v>361</v>
       </c>
     </row>
@@ -6259,7 +6262,7 @@
       <c r="E178" t="s">
         <v>362</v>
       </c>
-      <c r="F178" s="5" t="s">
+      <c r="F178" s="4" t="s">
         <v>363</v>
       </c>
     </row>
@@ -6279,7 +6282,7 @@
       <c r="E179" t="s">
         <v>364</v>
       </c>
-      <c r="F179" s="5" t="s">
+      <c r="F179" s="4" t="s">
         <v>365</v>
       </c>
     </row>
@@ -6299,7 +6302,7 @@
       <c r="E180" t="s">
         <v>366</v>
       </c>
-      <c r="F180" s="5" t="s">
+      <c r="F180" s="4" t="s">
         <v>367</v>
       </c>
     </row>
@@ -6319,7 +6322,7 @@
       <c r="E181" t="s">
         <v>368</v>
       </c>
-      <c r="F181" s="5" t="s">
+      <c r="F181" s="4" t="s">
         <v>369</v>
       </c>
     </row>
@@ -6339,7 +6342,7 @@
       <c r="E182" t="s">
         <v>370</v>
       </c>
-      <c r="F182" s="5" t="s">
+      <c r="F182" s="4" t="s">
         <v>371</v>
       </c>
     </row>
@@ -6359,7 +6362,7 @@
       <c r="E183" t="s">
         <v>372</v>
       </c>
-      <c r="F183" s="5" t="s">
+      <c r="F183" s="4" t="s">
         <v>373</v>
       </c>
     </row>
@@ -6379,7 +6382,7 @@
       <c r="E184" t="s">
         <v>374</v>
       </c>
-      <c r="F184" s="5" t="s">
+      <c r="F184" s="4" t="s">
         <v>375</v>
       </c>
     </row>
@@ -6399,7 +6402,7 @@
       <c r="E185" t="s">
         <v>376</v>
       </c>
-      <c r="F185" s="5" t="s">
+      <c r="F185" s="4" t="s">
         <v>377</v>
       </c>
     </row>
@@ -6419,7 +6422,7 @@
       <c r="E186" t="s">
         <v>378</v>
       </c>
-      <c r="F186" s="5" t="s">
+      <c r="F186" s="4" t="s">
         <v>379</v>
       </c>
     </row>
@@ -6439,7 +6442,7 @@
       <c r="E187" t="s">
         <v>380</v>
       </c>
-      <c r="F187" s="5" t="s">
+      <c r="F187" s="4" t="s">
         <v>381</v>
       </c>
     </row>
@@ -6459,7 +6462,7 @@
       <c r="E188" t="s">
         <v>382</v>
       </c>
-      <c r="F188" s="5" t="s">
+      <c r="F188" s="4" t="s">
         <v>383</v>
       </c>
     </row>
@@ -6479,7 +6482,7 @@
       <c r="E189" t="s">
         <v>384</v>
       </c>
-      <c r="F189" s="5" t="s">
+      <c r="F189" s="4" t="s">
         <v>385</v>
       </c>
     </row>
@@ -6499,7 +6502,7 @@
       <c r="E190" t="s">
         <v>386</v>
       </c>
-      <c r="F190" s="5" t="s">
+      <c r="F190" s="4" t="s">
         <v>387</v>
       </c>
     </row>
@@ -6519,7 +6522,7 @@
       <c r="E191" t="s">
         <v>388</v>
       </c>
-      <c r="F191" s="5" t="s">
+      <c r="F191" s="4" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6539,7 +6542,7 @@
       <c r="E192" t="s">
         <v>390</v>
       </c>
-      <c r="F192" s="5" t="s">
+      <c r="F192" s="4" t="s">
         <v>391</v>
       </c>
     </row>
@@ -6559,7 +6562,7 @@
       <c r="E193" t="s">
         <v>392</v>
       </c>
-      <c r="F193" s="5" t="s">
+      <c r="F193" s="4" t="s">
         <v>393</v>
       </c>
     </row>
@@ -6579,7 +6582,7 @@
       <c r="E194" t="s">
         <v>394</v>
       </c>
-      <c r="F194" s="5" t="s">
+      <c r="F194" s="4" t="s">
         <v>395</v>
       </c>
     </row>
@@ -6599,7 +6602,7 @@
       <c r="E195" t="s">
         <v>396</v>
       </c>
-      <c r="F195" s="5" t="s">
+      <c r="F195" s="4" t="s">
         <v>397</v>
       </c>
     </row>
@@ -6619,7 +6622,7 @@
       <c r="E196" t="s">
         <v>398</v>
       </c>
-      <c r="F196" s="5" t="s">
+      <c r="F196" s="4" t="s">
         <v>399</v>
       </c>
     </row>
@@ -6639,7 +6642,7 @@
       <c r="E197" t="s">
         <v>400</v>
       </c>
-      <c r="F197" s="5" t="s">
+      <c r="F197" s="4" t="s">
         <v>401</v>
       </c>
     </row>
@@ -6659,7 +6662,7 @@
       <c r="E198" t="s">
         <v>402</v>
       </c>
-      <c r="F198" s="5" t="s">
+      <c r="F198" s="4" t="s">
         <v>403</v>
       </c>
     </row>
@@ -6679,7 +6682,7 @@
       <c r="E199" t="s">
         <v>404</v>
       </c>
-      <c r="F199" s="5" t="s">
+      <c r="F199" s="4" t="s">
         <v>405</v>
       </c>
     </row>
@@ -6699,7 +6702,7 @@
       <c r="E200" t="s">
         <v>406</v>
       </c>
-      <c r="F200" s="5" t="s">
+      <c r="F200" s="4" t="s">
         <v>407</v>
       </c>
     </row>
@@ -6719,7 +6722,7 @@
       <c r="E201" t="s">
         <v>408</v>
       </c>
-      <c r="F201" s="5" t="s">
+      <c r="F201" s="4" t="s">
         <v>409</v>
       </c>
     </row>
@@ -6739,7 +6742,7 @@
       <c r="E202" t="s">
         <v>410</v>
       </c>
-      <c r="F202" s="5" t="s">
+      <c r="F202" s="4" t="s">
         <v>411</v>
       </c>
     </row>
@@ -6759,7 +6762,7 @@
       <c r="E203" t="s">
         <v>412</v>
       </c>
-      <c r="F203" s="5" t="s">
+      <c r="F203" s="4" t="s">
         <v>413</v>
       </c>
     </row>
@@ -6779,7 +6782,7 @@
       <c r="E204" t="s">
         <v>414</v>
       </c>
-      <c r="F204" s="5" t="s">
+      <c r="F204" s="4" t="s">
         <v>415</v>
       </c>
     </row>
@@ -6799,7 +6802,7 @@
       <c r="E205" t="s">
         <v>416</v>
       </c>
-      <c r="F205" s="5" t="s">
+      <c r="F205" s="4" t="s">
         <v>417</v>
       </c>
     </row>
@@ -6819,7 +6822,7 @@
       <c r="E206" t="s">
         <v>418</v>
       </c>
-      <c r="F206" s="5" t="s">
+      <c r="F206" s="4" t="s">
         <v>419</v>
       </c>
     </row>
@@ -6839,7 +6842,7 @@
       <c r="E207" t="s">
         <v>420</v>
       </c>
-      <c r="F207" s="5" t="s">
+      <c r="F207" s="4" t="s">
         <v>421</v>
       </c>
     </row>
@@ -6859,7 +6862,7 @@
       <c r="E208" t="s">
         <v>422</v>
       </c>
-      <c r="F208" s="5" t="s">
+      <c r="F208" s="4" t="s">
         <v>423</v>
       </c>
     </row>
@@ -6879,7 +6882,7 @@
       <c r="E209" t="s">
         <v>424</v>
       </c>
-      <c r="F209" s="5" t="s">
+      <c r="F209" s="4" t="s">
         <v>425</v>
       </c>
     </row>
@@ -6899,7 +6902,7 @@
       <c r="E210" t="s">
         <v>426</v>
       </c>
-      <c r="F210" s="5" t="s">
+      <c r="F210" s="4" t="s">
         <v>427</v>
       </c>
     </row>
@@ -6919,7 +6922,7 @@
       <c r="E211" t="s">
         <v>428</v>
       </c>
-      <c r="F211" s="5" t="s">
+      <c r="F211" s="4" t="s">
         <v>429</v>
       </c>
     </row>
@@ -6939,7 +6942,7 @@
       <c r="E212" t="s">
         <v>430</v>
       </c>
-      <c r="F212" s="5" t="s">
+      <c r="F212" s="4" t="s">
         <v>431</v>
       </c>
     </row>
@@ -6959,7 +6962,7 @@
       <c r="E213" t="s">
         <v>432</v>
       </c>
-      <c r="F213" s="5" t="s">
+      <c r="F213" s="4" t="s">
         <v>433</v>
       </c>
     </row>
@@ -6979,7 +6982,7 @@
       <c r="E214" t="s">
         <v>434</v>
       </c>
-      <c r="F214" s="5" t="s">
+      <c r="F214" s="4" t="s">
         <v>435</v>
       </c>
     </row>
@@ -6999,7 +7002,7 @@
       <c r="E215" t="s">
         <v>436</v>
       </c>
-      <c r="F215" s="5" t="s">
+      <c r="F215" s="4" t="s">
         <v>437</v>
       </c>
     </row>
@@ -7019,7 +7022,7 @@
       <c r="E216" t="s">
         <v>438</v>
       </c>
-      <c r="F216" s="5" t="s">
+      <c r="F216" s="4" t="s">
         <v>439</v>
       </c>
     </row>
@@ -7039,7 +7042,7 @@
       <c r="E217" t="s">
         <v>440</v>
       </c>
-      <c r="F217" s="5" t="s">
+      <c r="F217" s="4" t="s">
         <v>441</v>
       </c>
     </row>
@@ -7059,7 +7062,7 @@
       <c r="E218" t="s">
         <v>442</v>
       </c>
-      <c r="F218" s="5" t="s">
+      <c r="F218" s="4" t="s">
         <v>443</v>
       </c>
     </row>
@@ -7079,7 +7082,7 @@
       <c r="E219" t="s">
         <v>444</v>
       </c>
-      <c r="F219" s="5" t="s">
+      <c r="F219" s="4" t="s">
         <v>445</v>
       </c>
     </row>
@@ -7099,7 +7102,7 @@
       <c r="E220" t="s">
         <v>446</v>
       </c>
-      <c r="F220" s="5" t="s">
+      <c r="F220" s="4" t="s">
         <v>447</v>
       </c>
     </row>
@@ -7119,7 +7122,7 @@
       <c r="E221" t="s">
         <v>448</v>
       </c>
-      <c r="F221" s="5" t="s">
+      <c r="F221" s="4" t="s">
         <v>449</v>
       </c>
     </row>
@@ -7139,7 +7142,7 @@
       <c r="E222" t="s">
         <v>450</v>
       </c>
-      <c r="F222" s="5" t="s">
+      <c r="F222" s="4" t="s">
         <v>451</v>
       </c>
     </row>
@@ -7159,7 +7162,7 @@
       <c r="E223" t="s">
         <v>452</v>
       </c>
-      <c r="F223" s="5" t="s">
+      <c r="F223" s="4" t="s">
         <v>453</v>
       </c>
     </row>
@@ -7179,7 +7182,7 @@
       <c r="E224" t="s">
         <v>454</v>
       </c>
-      <c r="F224" s="5" t="s">
+      <c r="F224" s="4" t="s">
         <v>455</v>
       </c>
     </row>
@@ -7199,7 +7202,7 @@
       <c r="E225" t="s">
         <v>456</v>
       </c>
-      <c r="F225" s="5" t="s">
+      <c r="F225" s="4" t="s">
         <v>457</v>
       </c>
     </row>
@@ -7219,7 +7222,7 @@
       <c r="E226" t="s">
         <v>458</v>
       </c>
-      <c r="F226" s="5" t="s">
+      <c r="F226" s="4" t="s">
         <v>459</v>
       </c>
     </row>
@@ -7239,7 +7242,7 @@
       <c r="E227" t="s">
         <v>460</v>
       </c>
-      <c r="F227" s="5" t="s">
+      <c r="F227" s="4" t="s">
         <v>461</v>
       </c>
     </row>
@@ -7259,7 +7262,7 @@
       <c r="E228" t="s">
         <v>462</v>
       </c>
-      <c r="F228" s="5" t="s">
+      <c r="F228" s="4" t="s">
         <v>463</v>
       </c>
     </row>
@@ -7279,7 +7282,7 @@
       <c r="E229" t="s">
         <v>464</v>
       </c>
-      <c r="F229" s="5" t="s">
+      <c r="F229" s="4" t="s">
         <v>465</v>
       </c>
     </row>
@@ -7299,7 +7302,7 @@
       <c r="E230" t="s">
         <v>466</v>
       </c>
-      <c r="F230" s="5" t="s">
+      <c r="F230" s="4" t="s">
         <v>467</v>
       </c>
     </row>
@@ -7319,7 +7322,7 @@
       <c r="E231" t="s">
         <v>468</v>
       </c>
-      <c r="F231" s="5" t="s">
+      <c r="F231" s="4" t="s">
         <v>469</v>
       </c>
     </row>
@@ -7339,7 +7342,7 @@
       <c r="E232" t="s">
         <v>470</v>
       </c>
-      <c r="F232" s="5" t="s">
+      <c r="F232" s="4" t="s">
         <v>471</v>
       </c>
     </row>
@@ -7359,7 +7362,7 @@
       <c r="E233" t="s">
         <v>472</v>
       </c>
-      <c r="F233" s="5" t="s">
+      <c r="F233" s="4" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7379,7 +7382,7 @@
       <c r="E234" t="s">
         <v>474</v>
       </c>
-      <c r="F234" s="5" t="s">
+      <c r="F234" s="4" t="s">
         <v>475</v>
       </c>
     </row>
@@ -7399,7 +7402,7 @@
       <c r="E235" t="s">
         <v>476</v>
       </c>
-      <c r="F235" s="5" t="s">
+      <c r="F235" s="4" t="s">
         <v>477</v>
       </c>
     </row>
@@ -7419,7 +7422,7 @@
       <c r="E236" t="s">
         <v>478</v>
       </c>
-      <c r="F236" s="5" t="s">
+      <c r="F236" s="4" t="s">
         <v>479</v>
       </c>
     </row>
@@ -7439,7 +7442,7 @@
       <c r="E237" t="s">
         <v>480</v>
       </c>
-      <c r="F237" s="5" t="s">
+      <c r="F237" s="4" t="s">
         <v>481</v>
       </c>
     </row>
@@ -7459,7 +7462,7 @@
       <c r="E238" t="s">
         <v>482</v>
       </c>
-      <c r="F238" s="5" t="s">
+      <c r="F238" s="4" t="s">
         <v>483</v>
       </c>
     </row>
@@ -7479,7 +7482,7 @@
       <c r="E239" t="s">
         <v>484</v>
       </c>
-      <c r="F239" s="5" t="s">
+      <c r="F239" s="4" t="s">
         <v>485</v>
       </c>
     </row>
@@ -7499,7 +7502,7 @@
       <c r="E240" t="s">
         <v>486</v>
       </c>
-      <c r="F240" s="5" t="s">
+      <c r="F240" s="4" t="s">
         <v>487</v>
       </c>
     </row>
@@ -7519,7 +7522,7 @@
       <c r="E241" t="s">
         <v>488</v>
       </c>
-      <c r="F241" s="5" t="s">
+      <c r="F241" s="4" t="s">
         <v>489</v>
       </c>
     </row>
@@ -7539,7 +7542,7 @@
       <c r="E242" t="s">
         <v>490</v>
       </c>
-      <c r="F242" s="5" t="s">
+      <c r="F242" s="4" t="s">
         <v>491</v>
       </c>
     </row>
@@ -7559,7 +7562,7 @@
       <c r="E243" t="s">
         <v>492</v>
       </c>
-      <c r="F243" s="5" t="s">
+      <c r="F243" s="4" t="s">
         <v>493</v>
       </c>
     </row>
@@ -7579,7 +7582,7 @@
       <c r="E244" t="s">
         <v>494</v>
       </c>
-      <c r="F244" s="5" t="s">
+      <c r="F244" s="4" t="s">
         <v>495</v>
       </c>
     </row>
@@ -7599,7 +7602,7 @@
       <c r="E245" t="s">
         <v>496</v>
       </c>
-      <c r="F245" s="5" t="s">
+      <c r="F245" s="4" t="s">
         <v>497</v>
       </c>
     </row>
@@ -7619,7 +7622,7 @@
       <c r="E246" t="s">
         <v>498</v>
       </c>
-      <c r="F246" s="5" t="s">
+      <c r="F246" s="4" t="s">
         <v>499</v>
       </c>
     </row>
@@ -7639,7 +7642,7 @@
       <c r="E247" t="s">
         <v>500</v>
       </c>
-      <c r="F247" s="5" t="s">
+      <c r="F247" s="4" t="s">
         <v>501</v>
       </c>
     </row>
@@ -7659,7 +7662,7 @@
       <c r="E248" t="s">
         <v>502</v>
       </c>
-      <c r="F248" s="5" t="s">
+      <c r="F248" s="4" t="s">
         <v>503</v>
       </c>
     </row>
@@ -7679,7 +7682,7 @@
       <c r="E249" t="s">
         <v>504</v>
       </c>
-      <c r="F249" s="5" t="s">
+      <c r="F249" s="4" t="s">
         <v>505</v>
       </c>
     </row>
@@ -7699,7 +7702,7 @@
       <c r="E250" t="s">
         <v>506</v>
       </c>
-      <c r="F250" s="5" t="s">
+      <c r="F250" s="4" t="s">
         <v>507</v>
       </c>
     </row>
@@ -7719,7 +7722,7 @@
       <c r="E251" t="s">
         <v>508</v>
       </c>
-      <c r="F251" s="5" t="s">
+      <c r="F251" s="4" t="s">
         <v>509</v>
       </c>
     </row>
@@ -7739,7 +7742,7 @@
       <c r="E252" t="s">
         <v>510</v>
       </c>
-      <c r="F252" s="5" t="s">
+      <c r="F252" s="4" t="s">
         <v>511</v>
       </c>
     </row>
@@ -7759,7 +7762,7 @@
       <c r="E253" t="s">
         <v>512</v>
       </c>
-      <c r="F253" s="5" t="s">
+      <c r="F253" s="4" t="s">
         <v>513</v>
       </c>
     </row>
@@ -7779,7 +7782,7 @@
       <c r="E254" t="s">
         <v>514</v>
       </c>
-      <c r="F254" s="5" t="s">
+      <c r="F254" s="4" t="s">
         <v>515</v>
       </c>
     </row>
@@ -7799,7 +7802,7 @@
       <c r="E255" t="s">
         <v>516</v>
       </c>
-      <c r="F255" s="5" t="s">
+      <c r="F255" s="4" t="s">
         <v>517</v>
       </c>
     </row>
@@ -7819,11 +7822,11 @@
       <c r="E256" t="s">
         <v>518</v>
       </c>
-      <c r="F256" s="5" t="s">
+      <c r="F256" s="4" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="257" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>5</v>
       </c>
@@ -7839,11 +7842,11 @@
       <c r="E257" t="s">
         <v>520</v>
       </c>
-      <c r="F257" s="5" t="s">
+      <c r="F257" s="4" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="258" spans="1:7" ht="40" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>5</v>
       </c>
@@ -7859,11 +7862,11 @@
       <c r="E258" t="s">
         <v>522</v>
       </c>
-      <c r="F258" s="5" t="s">
+      <c r="F258" s="4" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="259" spans="1:7" ht="80" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>5</v>
       </c>
@@ -7879,11 +7882,11 @@
       <c r="E259" t="s">
         <v>524</v>
       </c>
-      <c r="F259" s="5" t="s">
+      <c r="F259" s="4" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="260" spans="1:7" ht="40" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>5</v>
       </c>
@@ -7899,11 +7902,11 @@
       <c r="E260" t="s">
         <v>526</v>
       </c>
-      <c r="F260" s="5" t="s">
+      <c r="F260" s="4" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="261" spans="1:7" ht="40" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>5</v>
       </c>
@@ -7919,11 +7922,11 @@
       <c r="E261" t="s">
         <v>528</v>
       </c>
-      <c r="F261" s="5" t="s">
+      <c r="F261" s="4" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="262" spans="1:7" ht="80" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>5</v>
       </c>
@@ -7939,11 +7942,11 @@
       <c r="E262" t="s">
         <v>530</v>
       </c>
-      <c r="F262" s="5" t="s">
+      <c r="F262" s="4" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="263" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>5</v>
       </c>
@@ -7959,11 +7962,11 @@
       <c r="E263" t="s">
         <v>532</v>
       </c>
-      <c r="F263" s="5" t="s">
+      <c r="F263" s="4" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="264" spans="1:7" ht="40" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>5</v>
       </c>
@@ -7979,11 +7982,11 @@
       <c r="E264" t="s">
         <v>534</v>
       </c>
-      <c r="F264" s="5" t="s">
+      <c r="F264" s="4" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="265" spans="1:7" ht="80" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>5</v>
       </c>
@@ -7999,11 +8002,11 @@
       <c r="E265" t="s">
         <v>536</v>
       </c>
-      <c r="F265" s="5" t="s">
+      <c r="F265" s="4" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="266" spans="1:7" ht="20" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>5</v>
       </c>
@@ -8019,11 +8022,11 @@
       <c r="E266" t="s">
         <v>538</v>
       </c>
-      <c r="F266" s="5" t="s">
+      <c r="F266" s="4" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="267" spans="1:7" ht="40" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>5</v>
       </c>
@@ -8039,14 +8042,18 @@
       <c r="E267" t="s">
         <v>540</v>
       </c>
-      <c r="F267" s="5" t="s">
+      <c r="F267" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="G267" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="268" spans="1:7" ht="40" x14ac:dyDescent="0.25">
+      <c r="G267" s="6">
+        <v>1</v>
+      </c>
+      <c r="M267">
+        <f t="shared" ref="M267:M330" si="0">G267</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>5</v>
       </c>
@@ -8062,14 +8069,18 @@
       <c r="E268" t="s">
         <v>542</v>
       </c>
-      <c r="F268" s="5" t="s">
+      <c r="F268" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="G268" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="269" spans="1:7" ht="40" x14ac:dyDescent="0.25">
+      <c r="G268" s="6">
+        <v>1</v>
+      </c>
+      <c r="M268">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>5</v>
       </c>
@@ -8085,14 +8096,18 @@
       <c r="E269" t="s">
         <v>544</v>
       </c>
-      <c r="F269" s="5" t="s">
+      <c r="F269" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="G269" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="270" spans="1:7" ht="40" x14ac:dyDescent="0.25">
+      <c r="G269" s="6">
+        <v>1</v>
+      </c>
+      <c r="M269">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>5</v>
       </c>
@@ -8108,14 +8123,18 @@
       <c r="E270" t="s">
         <v>546</v>
       </c>
-      <c r="F270" s="5" t="s">
+      <c r="F270" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="G270" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="271" spans="1:7" ht="80" x14ac:dyDescent="0.25">
+      <c r="G270" s="6">
+        <v>1</v>
+      </c>
+      <c r="M270">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>5</v>
       </c>
@@ -8131,14 +8150,18 @@
       <c r="E271" t="s">
         <v>548</v>
       </c>
-      <c r="F271" s="5" t="s">
+      <c r="F271" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="G271" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="272" spans="1:7" ht="40" x14ac:dyDescent="0.25">
+      <c r="G271" s="6">
+        <v>1</v>
+      </c>
+      <c r="M271">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>5</v>
       </c>
@@ -8154,14 +8177,18 @@
       <c r="E272" t="s">
         <v>550</v>
       </c>
-      <c r="F272" s="5" t="s">
+      <c r="F272" s="4" t="s">
         <v>551</v>
       </c>
       <c r="G272">
         <v>1</v>
       </c>
-    </row>
-    <row r="273" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="M272">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>5</v>
       </c>
@@ -8177,14 +8204,18 @@
       <c r="E273" t="s">
         <v>552</v>
       </c>
-      <c r="F273" s="5" t="s">
+      <c r="F273" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="G273" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="274" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G273" s="6">
+        <v>1</v>
+      </c>
+      <c r="M273">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>5</v>
       </c>
@@ -8200,14 +8231,18 @@
       <c r="E274" t="s">
         <v>554</v>
       </c>
-      <c r="F274" s="5" t="s">
+      <c r="F274" s="4" t="s">
         <v>555</v>
       </c>
-      <c r="G274" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="275" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G274" s="6">
+        <v>1</v>
+      </c>
+      <c r="M274">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>5</v>
       </c>
@@ -8223,14 +8258,18 @@
       <c r="E275" t="s">
         <v>556</v>
       </c>
-      <c r="F275" s="5" t="s">
+      <c r="F275" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="G275" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="276" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="G275" s="6">
+        <v>1</v>
+      </c>
+      <c r="M275">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>5</v>
       </c>
@@ -8246,14 +8285,18 @@
       <c r="E276" t="s">
         <v>558</v>
       </c>
-      <c r="F276" s="5" t="s">
+      <c r="F276" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="G276" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="277" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="G276" s="6">
+        <v>1</v>
+      </c>
+      <c r="M276">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>5</v>
       </c>
@@ -8269,14 +8312,18 @@
       <c r="E277" t="s">
         <v>560</v>
       </c>
-      <c r="F277" s="5" t="s">
+      <c r="F277" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="G277" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="278" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G277" s="6">
+        <v>1</v>
+      </c>
+      <c r="M277">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>5</v>
       </c>
@@ -8292,14 +8339,18 @@
       <c r="E278" t="s">
         <v>562</v>
       </c>
-      <c r="F278" s="5" t="s">
+      <c r="F278" s="4" t="s">
         <v>563</v>
       </c>
-      <c r="G278" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="279" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G278" s="6">
+        <v>1</v>
+      </c>
+      <c r="M278">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>5</v>
       </c>
@@ -8315,14 +8366,18 @@
       <c r="E279" t="s">
         <v>564</v>
       </c>
-      <c r="F279" s="5" t="s">
+      <c r="F279" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="G279" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="280" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G279" s="6">
+        <v>1</v>
+      </c>
+      <c r="M279">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>5</v>
       </c>
@@ -8338,14 +8393,18 @@
       <c r="E280" t="s">
         <v>566</v>
       </c>
-      <c r="F280" s="5" t="s">
+      <c r="F280" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="G280" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="281" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G280" s="6">
+        <v>1</v>
+      </c>
+      <c r="M280">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>5</v>
       </c>
@@ -8361,14 +8420,18 @@
       <c r="E281" t="s">
         <v>568</v>
       </c>
-      <c r="F281" s="5" t="s">
+      <c r="F281" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="G281" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="282" spans="1:11" ht="80" x14ac:dyDescent="0.25">
+      <c r="G281" s="6">
+        <v>1</v>
+      </c>
+      <c r="M281">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>5</v>
       </c>
@@ -8384,17 +8447,21 @@
       <c r="E282" t="s">
         <v>570</v>
       </c>
-      <c r="F282" s="5" t="s">
+      <c r="F282" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="G282" s="7">
+      <c r="G282" s="6">
         <v>0</v>
       </c>
       <c r="J282" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="283" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="M282">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>5</v>
       </c>
@@ -8410,14 +8477,18 @@
       <c r="E283" t="s">
         <v>572</v>
       </c>
-      <c r="F283" s="5" t="s">
+      <c r="F283" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="G283" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="284" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G283" s="6">
+        <v>1</v>
+      </c>
+      <c r="M283">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>5</v>
       </c>
@@ -8433,17 +8504,21 @@
       <c r="E284" t="s">
         <v>574</v>
       </c>
-      <c r="F284" s="5" t="s">
+      <c r="F284" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="G284" s="7">
+      <c r="G284" s="6">
         <v>0</v>
       </c>
       <c r="I284" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="285" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="M284">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>5</v>
       </c>
@@ -8459,14 +8534,18 @@
       <c r="E285" t="s">
         <v>576</v>
       </c>
-      <c r="F285" s="5" t="s">
+      <c r="F285" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="G285" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="286" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G285" s="6">
+        <v>1</v>
+      </c>
+      <c r="M285">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>5</v>
       </c>
@@ -8482,14 +8561,18 @@
       <c r="E286" t="s">
         <v>578</v>
       </c>
-      <c r="F286" s="5" t="s">
+      <c r="F286" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="G286" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="287" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="G286" s="6">
+        <v>1</v>
+      </c>
+      <c r="M286">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>5</v>
       </c>
@@ -8505,17 +8588,21 @@
       <c r="E287" t="s">
         <v>580</v>
       </c>
-      <c r="F287" s="5" t="s">
+      <c r="F287" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="G287" s="7">
+      <c r="G287" s="6">
         <v>0</v>
       </c>
       <c r="K287" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="288" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="M287">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>5</v>
       </c>
@@ -8531,14 +8618,18 @@
       <c r="E288" t="s">
         <v>582</v>
       </c>
-      <c r="F288" s="5" t="s">
+      <c r="F288" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="G288" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="289" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G288" s="6">
+        <v>1</v>
+      </c>
+      <c r="M288">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>5</v>
       </c>
@@ -8554,14 +8645,18 @@
       <c r="E289" t="s">
         <v>584</v>
       </c>
-      <c r="F289" s="5" t="s">
+      <c r="F289" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="G289" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="290" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="G289" s="6">
+        <v>1</v>
+      </c>
+      <c r="M289">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>5</v>
       </c>
@@ -8577,14 +8672,18 @@
       <c r="E290" t="s">
         <v>586</v>
       </c>
-      <c r="F290" s="5" t="s">
+      <c r="F290" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="G290" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="291" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G290" s="6">
+        <v>1</v>
+      </c>
+      <c r="M290">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>5</v>
       </c>
@@ -8600,14 +8699,18 @@
       <c r="E291" t="s">
         <v>588</v>
       </c>
-      <c r="F291" s="5" t="s">
+      <c r="F291" s="4" t="s">
         <v>589</v>
       </c>
-      <c r="G291" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="292" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G291" s="6">
+        <v>1</v>
+      </c>
+      <c r="M291">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>5</v>
       </c>
@@ -8623,14 +8726,18 @@
       <c r="E292" t="s">
         <v>590</v>
       </c>
-      <c r="F292" s="5" t="s">
+      <c r="F292" s="4" t="s">
         <v>591</v>
       </c>
-      <c r="G292" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="293" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="G292" s="6">
+        <v>1</v>
+      </c>
+      <c r="M292">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>5</v>
       </c>
@@ -8646,14 +8753,18 @@
       <c r="E293" t="s">
         <v>592</v>
       </c>
-      <c r="F293" s="5" t="s">
+      <c r="F293" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="G293" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="294" spans="1:11" ht="80" x14ac:dyDescent="0.25">
+      <c r="G293" s="6">
+        <v>1</v>
+      </c>
+      <c r="M293">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>5</v>
       </c>
@@ -8669,17 +8780,21 @@
       <c r="E294" t="s">
         <v>594</v>
       </c>
-      <c r="F294" s="5" t="s">
+      <c r="F294" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="G294" s="7">
+      <c r="G294" s="6">
         <v>0</v>
       </c>
       <c r="J294" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="295" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="M294">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>5</v>
       </c>
@@ -8695,14 +8810,18 @@
       <c r="E295" t="s">
         <v>596</v>
       </c>
-      <c r="F295" s="5" t="s">
+      <c r="F295" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="G295" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="296" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G295" s="6">
+        <v>1</v>
+      </c>
+      <c r="M295">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>5</v>
       </c>
@@ -8718,14 +8837,18 @@
       <c r="E296" t="s">
         <v>598</v>
       </c>
-      <c r="F296" s="5" t="s">
+      <c r="F296" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="G296" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="297" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G296" s="6">
+        <v>1</v>
+      </c>
+      <c r="M296">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>5</v>
       </c>
@@ -8741,14 +8864,18 @@
       <c r="E297" t="s">
         <v>600</v>
       </c>
-      <c r="F297" s="5" t="s">
+      <c r="F297" s="4" t="s">
         <v>601</v>
       </c>
-      <c r="G297" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="298" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G297" s="6">
+        <v>1</v>
+      </c>
+      <c r="M297">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>5</v>
       </c>
@@ -8764,17 +8891,21 @@
       <c r="E298" t="s">
         <v>602</v>
       </c>
-      <c r="F298" s="5" t="s">
+      <c r="F298" s="4" t="s">
         <v>603</v>
       </c>
-      <c r="G298" s="7">
+      <c r="G298" s="6">
         <v>0</v>
       </c>
       <c r="J298" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="299" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="M298">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>5</v>
       </c>
@@ -8790,14 +8921,18 @@
       <c r="E299" t="s">
         <v>604</v>
       </c>
-      <c r="F299" s="5" t="s">
+      <c r="F299" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="G299" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="300" spans="1:11" ht="80" x14ac:dyDescent="0.25">
+      <c r="G299" s="6">
+        <v>1</v>
+      </c>
+      <c r="M299">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>5</v>
       </c>
@@ -8813,14 +8948,18 @@
       <c r="E300" t="s">
         <v>606</v>
       </c>
-      <c r="F300" s="5" t="s">
+      <c r="F300" s="4" t="s">
         <v>607</v>
       </c>
-      <c r="G300" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="301" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G300" s="6">
+        <v>1</v>
+      </c>
+      <c r="M300">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>5</v>
       </c>
@@ -8836,14 +8975,18 @@
       <c r="E301" t="s">
         <v>608</v>
       </c>
-      <c r="F301" s="5" t="s">
+      <c r="F301" s="4" t="s">
         <v>609</v>
       </c>
-      <c r="G301" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="302" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G301" s="6">
+        <v>1</v>
+      </c>
+      <c r="M301">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>5</v>
       </c>
@@ -8859,14 +9002,18 @@
       <c r="E302" t="s">
         <v>610</v>
       </c>
-      <c r="F302" s="5" t="s">
+      <c r="F302" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="G302" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="303" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G302" s="6">
+        <v>1</v>
+      </c>
+      <c r="M302">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>5</v>
       </c>
@@ -8882,14 +9029,18 @@
       <c r="E303" t="s">
         <v>612</v>
       </c>
-      <c r="F303" s="5" t="s">
+      <c r="F303" s="4" t="s">
         <v>613</v>
       </c>
-      <c r="G303" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="304" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G303" s="6">
+        <v>1</v>
+      </c>
+      <c r="M303">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>5</v>
       </c>
@@ -8905,17 +9056,21 @@
       <c r="E304" t="s">
         <v>614</v>
       </c>
-      <c r="F304" s="5" t="s">
+      <c r="F304" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="G304" s="7">
+      <c r="G304" s="6">
         <v>0</v>
       </c>
       <c r="K304" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="305" spans="1:10" ht="40" x14ac:dyDescent="0.25">
+      <c r="M304">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>5</v>
       </c>
@@ -8931,14 +9086,18 @@
       <c r="E305" t="s">
         <v>616</v>
       </c>
-      <c r="F305" s="5" t="s">
+      <c r="F305" s="4" t="s">
         <v>617</v>
       </c>
-      <c r="G305" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="306" spans="1:10" ht="80" x14ac:dyDescent="0.25">
+      <c r="G305" s="6">
+        <v>1</v>
+      </c>
+      <c r="M305">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>5</v>
       </c>
@@ -8954,14 +9113,18 @@
       <c r="E306" t="s">
         <v>618</v>
       </c>
-      <c r="F306" s="5" t="s">
+      <c r="F306" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="G306" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="307" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="G306" s="6">
+        <v>1</v>
+      </c>
+      <c r="M306">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>5</v>
       </c>
@@ -8977,14 +9140,18 @@
       <c r="E307" t="s">
         <v>620</v>
       </c>
-      <c r="F307" s="5" t="s">
+      <c r="F307" s="4" t="s">
         <v>621</v>
       </c>
-      <c r="G307" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="308" spans="1:10" ht="40" x14ac:dyDescent="0.25">
+      <c r="G307" s="6">
+        <v>1</v>
+      </c>
+      <c r="M307">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>5</v>
       </c>
@@ -9000,14 +9167,18 @@
       <c r="E308" t="s">
         <v>622</v>
       </c>
-      <c r="F308" s="5" t="s">
+      <c r="F308" s="4" t="s">
         <v>623</v>
       </c>
-      <c r="G308" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="309" spans="1:10" ht="40" x14ac:dyDescent="0.25">
+      <c r="G308" s="6">
+        <v>1</v>
+      </c>
+      <c r="M308">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>5</v>
       </c>
@@ -9023,14 +9194,18 @@
       <c r="E309" t="s">
         <v>624</v>
       </c>
-      <c r="F309" s="5" t="s">
+      <c r="F309" s="4" t="s">
         <v>625</v>
       </c>
-      <c r="G309" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="310" spans="1:10" ht="80" x14ac:dyDescent="0.25">
+      <c r="G309" s="6">
+        <v>1</v>
+      </c>
+      <c r="M309">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>5</v>
       </c>
@@ -9046,14 +9221,18 @@
       <c r="E310" t="s">
         <v>626</v>
       </c>
-      <c r="F310" s="5" t="s">
+      <c r="F310" s="4" t="s">
         <v>627</v>
       </c>
-      <c r="G310" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="311" spans="1:10" ht="40" x14ac:dyDescent="0.25">
+      <c r="G310" s="6">
+        <v>1</v>
+      </c>
+      <c r="M310">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>5</v>
       </c>
@@ -9069,14 +9248,18 @@
       <c r="E311" t="s">
         <v>628</v>
       </c>
-      <c r="F311" s="5" t="s">
+      <c r="F311" s="4" t="s">
         <v>629</v>
       </c>
-      <c r="G311" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="312" spans="1:10" ht="40" x14ac:dyDescent="0.25">
+      <c r="G311" s="6">
+        <v>1</v>
+      </c>
+      <c r="M311">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>5</v>
       </c>
@@ -9092,14 +9275,18 @@
       <c r="E312" t="s">
         <v>630</v>
       </c>
-      <c r="F312" s="5" t="s">
+      <c r="F312" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="G312" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="313" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="G312" s="6">
+        <v>1</v>
+      </c>
+      <c r="M312">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>5</v>
       </c>
@@ -9115,14 +9302,18 @@
       <c r="E313" t="s">
         <v>632</v>
       </c>
-      <c r="F313" s="5" t="s">
+      <c r="F313" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="G313" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="314" spans="1:10" ht="40" x14ac:dyDescent="0.25">
+      <c r="G313" s="6">
+        <v>1</v>
+      </c>
+      <c r="M313">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>5</v>
       </c>
@@ -9138,14 +9329,18 @@
       <c r="E314" t="s">
         <v>634</v>
       </c>
-      <c r="F314" s="5" t="s">
+      <c r="F314" s="4" t="s">
         <v>635</v>
       </c>
-      <c r="G314" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="315" spans="1:10" ht="40" x14ac:dyDescent="0.25">
+      <c r="G314" s="6">
+        <v>1</v>
+      </c>
+      <c r="M314">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>5</v>
       </c>
@@ -9161,14 +9356,18 @@
       <c r="E315" t="s">
         <v>636</v>
       </c>
-      <c r="F315" s="5" t="s">
+      <c r="F315" s="4" t="s">
         <v>637</v>
       </c>
-      <c r="G315" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="316" spans="1:10" ht="20" x14ac:dyDescent="0.25">
+      <c r="G315" s="6">
+        <v>1</v>
+      </c>
+      <c r="M315">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>5</v>
       </c>
@@ -9184,14 +9383,18 @@
       <c r="E316" t="s">
         <v>638</v>
       </c>
-      <c r="F316" s="5" t="s">
+      <c r="F316" s="4" t="s">
         <v>639</v>
       </c>
-      <c r="G316" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="317" spans="1:10" ht="40" x14ac:dyDescent="0.25">
+      <c r="G316" s="6">
+        <v>1</v>
+      </c>
+      <c r="M316">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>5</v>
       </c>
@@ -9207,14 +9410,18 @@
       <c r="E317" t="s">
         <v>640</v>
       </c>
-      <c r="F317" s="5" t="s">
+      <c r="F317" s="4" t="s">
         <v>641</v>
       </c>
-      <c r="G317" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="318" spans="1:10" ht="40" x14ac:dyDescent="0.25">
+      <c r="G317" s="6">
+        <v>1</v>
+      </c>
+      <c r="M317">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>5</v>
       </c>
@@ -9230,14 +9437,18 @@
       <c r="E318" t="s">
         <v>642</v>
       </c>
-      <c r="F318" s="5" t="s">
+      <c r="F318" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="G318" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="319" spans="1:10" ht="40" x14ac:dyDescent="0.25">
+      <c r="G318" s="6">
+        <v>1</v>
+      </c>
+      <c r="M318">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>5</v>
       </c>
@@ -9253,17 +9464,21 @@
       <c r="E319" t="s">
         <v>644</v>
       </c>
-      <c r="F319" s="5" t="s">
+      <c r="F319" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="G319" s="7">
+      <c r="G319" s="6">
         <v>0</v>
       </c>
       <c r="J319" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="320" spans="1:10" ht="40" x14ac:dyDescent="0.25">
+      <c r="M319">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>5</v>
       </c>
@@ -9279,14 +9494,18 @@
       <c r="E320" t="s">
         <v>646</v>
       </c>
-      <c r="F320" s="5" t="s">
+      <c r="F320" s="4" t="s">
         <v>647</v>
       </c>
-      <c r="G320" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="321" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="G320" s="6">
+        <v>1</v>
+      </c>
+      <c r="M320">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>5</v>
       </c>
@@ -9302,14 +9521,18 @@
       <c r="E321" t="s">
         <v>648</v>
       </c>
-      <c r="F321" s="5" t="s">
+      <c r="F321" s="4" t="s">
         <v>649</v>
       </c>
-      <c r="G321" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="322" spans="1:9" ht="20" x14ac:dyDescent="0.25">
+      <c r="G321" s="6">
+        <v>1</v>
+      </c>
+      <c r="M321">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>5</v>
       </c>
@@ -9325,14 +9548,18 @@
       <c r="E322" t="s">
         <v>650</v>
       </c>
-      <c r="F322" s="5" t="s">
+      <c r="F322" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="G322" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="323" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="G322" s="6">
+        <v>1</v>
+      </c>
+      <c r="M322">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>5</v>
       </c>
@@ -9348,14 +9575,18 @@
       <c r="E323" t="s">
         <v>652</v>
       </c>
-      <c r="F323" s="5" t="s">
+      <c r="F323" s="4" t="s">
         <v>653</v>
       </c>
-      <c r="G323" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="324" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="G323" s="6">
+        <v>1</v>
+      </c>
+      <c r="M323">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>5</v>
       </c>
@@ -9371,14 +9602,18 @@
       <c r="E324" t="s">
         <v>654</v>
       </c>
-      <c r="F324" s="5" t="s">
+      <c r="F324" s="4" t="s">
         <v>655</v>
       </c>
-      <c r="G324" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="325" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="G324" s="6">
+        <v>1</v>
+      </c>
+      <c r="M324">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>5</v>
       </c>
@@ -9394,14 +9629,18 @@
       <c r="E325" t="s">
         <v>656</v>
       </c>
-      <c r="F325" s="5" t="s">
+      <c r="F325" s="4" t="s">
         <v>657</v>
       </c>
-      <c r="G325" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="326" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="G325" s="6">
+        <v>1</v>
+      </c>
+      <c r="M325">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>5</v>
       </c>
@@ -9417,14 +9656,18 @@
       <c r="E326" t="s">
         <v>658</v>
       </c>
-      <c r="F326" s="5" t="s">
+      <c r="F326" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="G326" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="327" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="G326" s="6">
+        <v>1</v>
+      </c>
+      <c r="M326">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>5</v>
       </c>
@@ -9440,14 +9683,18 @@
       <c r="E327" t="s">
         <v>660</v>
       </c>
-      <c r="F327" s="5" t="s">
+      <c r="F327" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="G327" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="328" spans="1:9" ht="20" x14ac:dyDescent="0.25">
+      <c r="G327" s="6">
+        <v>1</v>
+      </c>
+      <c r="M327">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>5</v>
       </c>
@@ -9463,14 +9710,18 @@
       <c r="E328" t="s">
         <v>662</v>
       </c>
-      <c r="F328" s="5" t="s">
+      <c r="F328" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="G328" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="329" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="G328" s="6">
+        <v>1</v>
+      </c>
+      <c r="M328">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>5</v>
       </c>
@@ -9486,14 +9737,18 @@
       <c r="E329" t="s">
         <v>664</v>
       </c>
-      <c r="F329" s="5" t="s">
+      <c r="F329" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="G329" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="330" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="G329" s="6">
+        <v>1</v>
+      </c>
+      <c r="M329">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>5</v>
       </c>
@@ -9509,17 +9764,21 @@
       <c r="E330" t="s">
         <v>666</v>
       </c>
-      <c r="F330" s="5" t="s">
+      <c r="F330" s="4" t="s">
         <v>667</v>
       </c>
-      <c r="G330" s="7">
+      <c r="G330" s="6">
         <v>0</v>
       </c>
       <c r="I330" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="331" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="M330">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>5</v>
       </c>
@@ -9535,14 +9794,18 @@
       <c r="E331" t="s">
         <v>668</v>
       </c>
-      <c r="F331" s="5" t="s">
+      <c r="F331" s="4" t="s">
         <v>669</v>
       </c>
-      <c r="G331" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="332" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="G331" s="6">
+        <v>1</v>
+      </c>
+      <c r="M331">
+        <f t="shared" ref="M331:M355" si="1">G331</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>5</v>
       </c>
@@ -9558,14 +9821,18 @@
       <c r="E332" t="s">
         <v>670</v>
       </c>
-      <c r="F332" s="5" t="s">
+      <c r="F332" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="G332" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="333" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="G332" s="6">
+        <v>1</v>
+      </c>
+      <c r="M332">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>5</v>
       </c>
@@ -9581,14 +9848,18 @@
       <c r="E333" t="s">
         <v>672</v>
       </c>
-      <c r="F333" s="5" t="s">
+      <c r="F333" s="4" t="s">
         <v>673</v>
       </c>
-      <c r="G333" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="334" spans="1:9" ht="100" x14ac:dyDescent="0.25">
+      <c r="G333" s="6">
+        <v>1</v>
+      </c>
+      <c r="M333">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334" spans="1:13" ht="100" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>5</v>
       </c>
@@ -9604,14 +9875,18 @@
       <c r="E334" t="s">
         <v>674</v>
       </c>
-      <c r="F334" s="5" t="s">
+      <c r="F334" s="4" t="s">
         <v>675</v>
       </c>
-      <c r="G334" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="335" spans="1:9" ht="20" x14ac:dyDescent="0.25">
+      <c r="G334" s="6">
+        <v>1</v>
+      </c>
+      <c r="M334">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>5</v>
       </c>
@@ -9627,14 +9902,18 @@
       <c r="E335" t="s">
         <v>676</v>
       </c>
-      <c r="F335" s="5" t="s">
+      <c r="F335" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="G335" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="336" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="G335" s="6">
+        <v>1</v>
+      </c>
+      <c r="M335">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>5</v>
       </c>
@@ -9650,14 +9929,18 @@
       <c r="E336" t="s">
         <v>678</v>
       </c>
-      <c r="F336" s="5" t="s">
+      <c r="F336" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="G336" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="337" spans="1:11" ht="80" x14ac:dyDescent="0.25">
+      <c r="G336" s="6">
+        <v>1</v>
+      </c>
+      <c r="M336">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>5</v>
       </c>
@@ -9673,17 +9956,21 @@
       <c r="E337" t="s">
         <v>680</v>
       </c>
-      <c r="F337" s="5" t="s">
+      <c r="F337" s="4" t="s">
         <v>681</v>
       </c>
-      <c r="G337" s="7">
+      <c r="G337" s="6">
         <v>0</v>
       </c>
       <c r="I337" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="338" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="M337">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>5</v>
       </c>
@@ -9699,14 +9986,18 @@
       <c r="E338" t="s">
         <v>682</v>
       </c>
-      <c r="F338" s="5" t="s">
+      <c r="F338" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="G338" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="339" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G338" s="6">
+        <v>1</v>
+      </c>
+      <c r="M338">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>5</v>
       </c>
@@ -9722,14 +10013,18 @@
       <c r="E339" t="s">
         <v>684</v>
       </c>
-      <c r="F339" s="5" t="s">
+      <c r="F339" s="4" t="s">
         <v>685</v>
       </c>
-      <c r="G339" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="340" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G339" s="6">
+        <v>1</v>
+      </c>
+      <c r="M339">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>5</v>
       </c>
@@ -9745,14 +10040,18 @@
       <c r="E340" t="s">
         <v>686</v>
       </c>
-      <c r="F340" s="5" t="s">
+      <c r="F340" s="4" t="s">
         <v>687</v>
       </c>
-      <c r="G340" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="341" spans="1:11" ht="80" x14ac:dyDescent="0.25">
+      <c r="G340" s="6">
+        <v>1</v>
+      </c>
+      <c r="M340">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>5</v>
       </c>
@@ -9768,14 +10067,18 @@
       <c r="E341" t="s">
         <v>688</v>
       </c>
-      <c r="F341" s="5" t="s">
+      <c r="F341" s="4" t="s">
         <v>689</v>
       </c>
-      <c r="G341" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="342" spans="1:11" ht="80" x14ac:dyDescent="0.25">
+      <c r="G341" s="6">
+        <v>1</v>
+      </c>
+      <c r="M341">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>5</v>
       </c>
@@ -9791,14 +10094,18 @@
       <c r="E342" t="s">
         <v>690</v>
       </c>
-      <c r="F342" s="5" t="s">
+      <c r="F342" s="4" t="s">
         <v>691</v>
       </c>
-      <c r="G342" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="343" spans="1:11" ht="80" x14ac:dyDescent="0.25">
+      <c r="G342" s="6">
+        <v>1</v>
+      </c>
+      <c r="M342">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" ht="80" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>5</v>
       </c>
@@ -9814,14 +10121,18 @@
       <c r="E343" t="s">
         <v>692</v>
       </c>
-      <c r="F343" s="5" t="s">
+      <c r="F343" s="4" t="s">
         <v>693</v>
       </c>
-      <c r="G343" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="344" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G343" s="6">
+        <v>1</v>
+      </c>
+      <c r="M343">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>5</v>
       </c>
@@ -9837,14 +10148,18 @@
       <c r="E344" t="s">
         <v>694</v>
       </c>
-      <c r="F344" s="5" t="s">
+      <c r="F344" s="4" t="s">
         <v>695</v>
       </c>
-      <c r="G344" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="345" spans="1:11" ht="20" x14ac:dyDescent="0.25">
+      <c r="G344" s="6">
+        <v>1</v>
+      </c>
+      <c r="M344">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:13" ht="20" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>5</v>
       </c>
@@ -9860,14 +10175,18 @@
       <c r="E345" t="s">
         <v>696</v>
       </c>
-      <c r="F345" s="5" t="s">
+      <c r="F345" s="4" t="s">
         <v>697</v>
       </c>
-      <c r="G345" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="346" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G345" s="6">
+        <v>1</v>
+      </c>
+      <c r="M345">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>5</v>
       </c>
@@ -9883,14 +10202,18 @@
       <c r="E346" t="s">
         <v>698</v>
       </c>
-      <c r="F346" s="5" t="s">
+      <c r="F346" s="4" t="s">
         <v>699</v>
       </c>
-      <c r="G346" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="347" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G346" s="6">
+        <v>1</v>
+      </c>
+      <c r="M346">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>5</v>
       </c>
@@ -9906,14 +10229,18 @@
       <c r="E347" t="s">
         <v>700</v>
       </c>
-      <c r="F347" s="5" t="s">
+      <c r="F347" s="4" t="s">
         <v>701</v>
       </c>
-      <c r="G347" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="348" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G347" s="6">
+        <v>1</v>
+      </c>
+      <c r="M347">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="348" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>5</v>
       </c>
@@ -9929,14 +10256,18 @@
       <c r="E348" t="s">
         <v>702</v>
       </c>
-      <c r="F348" s="5" t="s">
+      <c r="F348" s="4" t="s">
         <v>703</v>
       </c>
-      <c r="G348" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="349" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G348" s="6">
+        <v>1</v>
+      </c>
+      <c r="M348">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>5</v>
       </c>
@@ -9952,17 +10283,21 @@
       <c r="E349" t="s">
         <v>704</v>
       </c>
-      <c r="F349" s="5" t="s">
+      <c r="F349" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="G349" s="7">
+      <c r="G349" s="6">
         <v>0</v>
       </c>
       <c r="K349" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="350" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="M349">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>5</v>
       </c>
@@ -9978,14 +10313,18 @@
       <c r="E350" t="s">
         <v>706</v>
       </c>
-      <c r="F350" s="5" t="s">
+      <c r="F350" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="G350" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="351" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="G350" s="6">
+        <v>1</v>
+      </c>
+      <c r="M350">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>5</v>
       </c>
@@ -10001,14 +10340,18 @@
       <c r="E351" t="s">
         <v>708</v>
       </c>
-      <c r="F351" s="5" t="s">
+      <c r="F351" s="4" t="s">
         <v>709</v>
       </c>
-      <c r="G351" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="352" spans="1:11" ht="40" x14ac:dyDescent="0.25">
+      <c r="G351" s="6">
+        <v>1</v>
+      </c>
+      <c r="M351">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>5</v>
       </c>
@@ -10024,14 +10367,18 @@
       <c r="E352" t="s">
         <v>710</v>
       </c>
-      <c r="F352" s="5" t="s">
+      <c r="F352" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="G352" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="353" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="G352" s="6">
+        <v>1</v>
+      </c>
+      <c r="M352">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>5</v>
       </c>
@@ -10047,10 +10394,10 @@
       <c r="E353" t="s">
         <v>712</v>
       </c>
-      <c r="F353" s="5" t="s">
+      <c r="F353" s="4" t="s">
         <v>713</v>
       </c>
-      <c r="G353" s="7">
+      <c r="G353" s="6">
         <v>0</v>
       </c>
       <c r="J353" t="s">
@@ -10059,8 +10406,12 @@
       <c r="L353" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="354" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+      <c r="M353">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>5</v>
       </c>
@@ -10076,14 +10427,18 @@
       <c r="E354" t="s">
         <v>714</v>
       </c>
-      <c r="F354" s="5" t="s">
+      <c r="F354" s="4" t="s">
         <v>715</v>
       </c>
-      <c r="G354" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="355" spans="1:12" ht="40" x14ac:dyDescent="0.25">
+      <c r="G354" s="6">
+        <v>1</v>
+      </c>
+      <c r="M354">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="1:13" ht="40" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>5</v>
       </c>
@@ -10099,14 +10454,18 @@
       <c r="E355" t="s">
         <v>716</v>
       </c>
-      <c r="F355" s="5" t="s">
+      <c r="F355" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="G355" s="7">
+      <c r="G355" s="6">
         <v>0</v>
       </c>
       <c r="K355" t="s">
         <v>724</v>
+      </c>
+      <c r="M355">
+        <f>G355</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>